<commit_message>
Update digikey part for fram chip
</commit_message>
<xml_diff>
--- a/hardware/controller/rev_a/controller_bom.xlsx
+++ b/hardware/controller/rev_a/controller_bom.xlsx
@@ -674,9 +674,6 @@
     <t>Cypress FRAM</t>
   </si>
   <si>
-    <t>428-3206-ND</t>
-  </si>
-  <si>
     <t>U5</t>
   </si>
   <si>
@@ -792,6 +789,9 @@
   </si>
   <si>
     <t>300Ohm</t>
+  </si>
+  <si>
+    <t>FM25CL64B-DGRA-ND</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1125,7 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,7 +1847,7 @@
         <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C36" t="s">
         <v>74</v>
@@ -1864,7 +1864,7 @@
         <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C37" t="s">
         <v>77</v>
@@ -1881,7 +1881,7 @@
         <v>79</v>
       </c>
       <c r="B38" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C38" t="s">
         <v>74</v>
@@ -1898,7 +1898,7 @@
         <v>81</v>
       </c>
       <c r="B39" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C39" t="s">
         <v>74</v>
@@ -2222,7 +2222,7 @@
         <v>143</v>
       </c>
       <c r="B57" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C57" t="s">
         <v>144</v>
@@ -2242,7 +2242,7 @@
         <v>148</v>
       </c>
       <c r="B58" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C58" t="s">
         <v>144</v>
@@ -2262,7 +2262,7 @@
         <v>149</v>
       </c>
       <c r="B59" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C59" t="s">
         <v>144</v>
@@ -2282,7 +2282,7 @@
         <v>151</v>
       </c>
       <c r="B60" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C60" t="s">
         <v>144</v>
@@ -2302,7 +2302,7 @@
         <v>152</v>
       </c>
       <c r="B61" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C61" t="s">
         <v>144</v>
@@ -2322,7 +2322,7 @@
         <v>154</v>
       </c>
       <c r="B62" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C62" t="s">
         <v>144</v>
@@ -2342,7 +2342,7 @@
         <v>155</v>
       </c>
       <c r="B63" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C63" t="s">
         <v>144</v>
@@ -2362,7 +2362,7 @@
         <v>156</v>
       </c>
       <c r="B64" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C64" t="s">
         <v>144</v>
@@ -2382,7 +2382,7 @@
         <v>157</v>
       </c>
       <c r="B65" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C65" t="s">
         <v>144</v>
@@ -2402,7 +2402,7 @@
         <v>158</v>
       </c>
       <c r="B66" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C66" t="s">
         <v>144</v>
@@ -2422,7 +2422,7 @@
         <v>159</v>
       </c>
       <c r="B67" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C67" t="s">
         <v>144</v>
@@ -2442,7 +2442,7 @@
         <v>161</v>
       </c>
       <c r="B68" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C68" t="s">
         <v>144</v>
@@ -2462,7 +2462,7 @@
         <v>162</v>
       </c>
       <c r="B69" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C69" t="s">
         <v>144</v>
@@ -2482,7 +2482,7 @@
         <v>163</v>
       </c>
       <c r="B70" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C70" t="s">
         <v>144</v>
@@ -2502,7 +2502,7 @@
         <v>164</v>
       </c>
       <c r="B71" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C71" t="s">
         <v>144</v>
@@ -2522,7 +2522,7 @@
         <v>165</v>
       </c>
       <c r="B72" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C72" t="s">
         <v>144</v>
@@ -2542,7 +2542,7 @@
         <v>166</v>
       </c>
       <c r="B73" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C73" t="s">
         <v>144</v>
@@ -2562,7 +2562,7 @@
         <v>168</v>
       </c>
       <c r="B74" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C74" t="s">
         <v>144</v>
@@ -2582,7 +2582,7 @@
         <v>169</v>
       </c>
       <c r="B75" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C75" t="s">
         <v>144</v>
@@ -2602,7 +2602,7 @@
         <v>170</v>
       </c>
       <c r="B76" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C76" t="s">
         <v>144</v>
@@ -2622,7 +2622,7 @@
         <v>171</v>
       </c>
       <c r="B77" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C77" t="s">
         <v>144</v>
@@ -2642,7 +2642,7 @@
         <v>172</v>
       </c>
       <c r="B78" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C78" t="s">
         <v>144</v>
@@ -2662,7 +2662,7 @@
         <v>174</v>
       </c>
       <c r="B79" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C79" t="s">
         <v>144</v>
@@ -2682,7 +2682,7 @@
         <v>176</v>
       </c>
       <c r="B80" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C80" t="s">
         <v>144</v>
@@ -2845,130 +2845,130 @@
         <v>207</v>
       </c>
       <c r="G88" t="s">
-        <v>208</v>
+        <v>247</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>208</v>
+      </c>
+      <c r="B89" t="s">
         <v>209</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
+        <v>209</v>
+      </c>
+      <c r="D89" t="s">
         <v>210</v>
       </c>
-      <c r="C89" t="s">
-        <v>210</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
         <v>211</v>
       </c>
-      <c r="E89" t="s">
+      <c r="G89" t="s">
         <v>212</v>
-      </c>
-      <c r="G89" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>213</v>
+      </c>
+      <c r="B90" t="s">
         <v>214</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
+        <v>214</v>
+      </c>
+      <c r="D90" t="s">
         <v>215</v>
       </c>
-      <c r="C90" t="s">
-        <v>215</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
         <v>216</v>
       </c>
-      <c r="E90" t="s">
+      <c r="G90" t="s">
         <v>217</v>
       </c>
-      <c r="G90" t="s">
+      <c r="H90" t="s">
         <v>218</v>
-      </c>
-      <c r="H90" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>219</v>
+      </c>
+      <c r="B91" t="s">
         <v>220</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
+        <v>220</v>
+      </c>
+      <c r="D91" t="s">
         <v>221</v>
       </c>
-      <c r="C91" t="s">
-        <v>221</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>222</v>
       </c>
-      <c r="E91" t="s">
+      <c r="G91" t="s">
         <v>223</v>
-      </c>
-      <c r="G91" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>224</v>
+      </c>
+      <c r="B92" t="s">
         <v>225</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
+        <v>225</v>
+      </c>
+      <c r="D92" t="s">
         <v>226</v>
       </c>
-      <c r="C92" t="s">
-        <v>226</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>227</v>
       </c>
-      <c r="E92" t="s">
+      <c r="G92" t="s">
         <v>228</v>
-      </c>
-      <c r="G92" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>229</v>
+      </c>
+      <c r="B93" t="s">
         <v>230</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
         <v>231</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>232</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>233</v>
       </c>
-      <c r="E93" t="s">
+      <c r="G93" t="s">
         <v>234</v>
-      </c>
-      <c r="G93" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B94" t="s">
+        <v>230</v>
+      </c>
+      <c r="C94" t="s">
         <v>231</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>232</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>233</v>
       </c>
-      <c r="E94" t="s">
+      <c r="G94" t="s">
         <v>234</v>
-      </c>
-      <c r="G94" t="s">
-        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final touches on controller
</commit_message>
<xml_diff>
--- a/hardware/controller/rev_a/controller_bom.xlsx
+++ b/hardware/controller/rev_a/controller_bom.xlsx
@@ -16,6 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="controller_bom" localSheetId="0">Sheet1!$A$1:$K$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$46</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -689,10 +690,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -982,8 +990,8 @@
   </sheetPr>
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,15 +999,15 @@
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1034,1043 +1042,1043 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2" t="s">
+    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2" t="s">
+      <c r="H12" s="3"/>
+      <c r="I12" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>2</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>2</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>2</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="21" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
+    <row r="22" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
+    <row r="23" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>2</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="25" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>2</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>1212</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="27" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="28" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="29" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>2</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="30" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>2</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="31" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>6</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="32" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>6</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="33" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>5</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>1</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="34" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>1</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="35" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>1</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="36" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>1</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="37" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>1</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="K37" t="s">
+      <c r="K37" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="38" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>1</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="39" spans="1:11" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
         <v>2</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="40" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>1</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>1</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="41" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>1</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="42" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>1</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="B43" t="s">
+    <row r="43" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>1</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J43" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44" t="s">
+    <row r="44" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>1</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="45" spans="1:11" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>1</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="46" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
         <v>2</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2078,7 +2086,7 @@
   <sortState ref="A2:K49">
     <sortCondition ref="E2:E49"/>
   </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="35" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="49" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>